<commit_message>
machine unique minimiser durée en jours - légende
</commit_message>
<xml_diff>
--- a/26. Excel - Recherche opérationnelle linéaire/37 - ORDONNANCEMENT - UNE MACHINE AVEC JOB EN RETARD/Jobshop(1).xlsx
+++ b/26. Excel - Recherche opérationnelle linéaire/37 - ORDONNANCEMENT - UNE MACHINE AVEC JOB EN RETARD/Jobshop(1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\python-data-science2\26. Recherche opérationnelle en Excel\37 - JOB SHOP - JOB SHOP SUR UNE MACHINE AVEC JOB EN RETARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\python-data-science2\26. Excel - Recherche opérationnelle linéaire\37 - ORDONNANCEMENT - UNE MACHINE AVEC JOB EN RETARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -79,7 +79,7 @@
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Job</t>
   </si>
@@ -117,6 +117,21 @@
   <si>
     <t>Days Late</t>
   </si>
+  <si>
+    <t>val 2:5</t>
+  </si>
+  <si>
+    <t>val 11:9</t>
+  </si>
+  <si>
+    <t>val 8:3</t>
+  </si>
+  <si>
+    <t>val etc…</t>
+  </si>
+  <si>
+    <t>Ordonnancement trouvé :</t>
+  </si>
 </sst>
 </file>
 
@@ -138,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +163,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,10 +197,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +522,7 @@
   <dimension ref="E1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -905,10 +942,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:L16"/>
+  <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,19 +1011,19 @@
       <c r="H5" s="2">
         <v>2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <f t="shared" ref="I5:I16" si="0">VLOOKUP(H5,lookup,2)</f>
         <v>5</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <f t="shared" ref="J5:J16" si="1">VLOOKUP(H5,lookup,3)</f>
         <v>33</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <f>I5</f>
         <v>5</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <f>IF(K5&gt;J5,K5-J5,0)</f>
         <v>0</v>
       </c>
@@ -1004,19 +1041,19 @@
       <c r="H6" s="2">
         <v>11</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <f>K5+I6</f>
         <v>14</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <f t="shared" ref="L6:L16" si="2">IF(K6&gt;J6,K6-J6,0)</f>
         <v>0</v>
       </c>
@@ -1034,19 +1071,19 @@
       <c r="H7" s="2">
         <v>8</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J7">
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J7" s="6">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="6">
         <f t="shared" ref="K7:K16" si="3">K6+I7</f>
         <v>17</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1319,6 +1356,25 @@
       <c r="L16">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>